<commit_message>
Table sent to HTML
</commit_message>
<xml_diff>
--- a/archivos/factura.xlsx
+++ b/archivos/factura.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qr362ep\GitHub\factura\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA00D4C-BC47-497B-9073-B877A60471D3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53BA3EE-52D3-415B-ADFD-0C030020B8EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>Resource Name</t>
   </si>
@@ -152,22 +152,7 @@
     <t>Business Unit</t>
   </si>
   <si>
-    <t>ComRes</t>
-  </si>
-  <si>
     <t>AutoSol</t>
-  </si>
-  <si>
-    <t>Corporate</t>
-  </si>
-  <si>
-    <t>Flow</t>
-  </si>
-  <si>
-    <t>Bill Blaise</t>
-  </si>
-  <si>
-    <t>n/a</t>
   </si>
   <si>
     <t>Diana García</t>
@@ -185,13 +170,7 @@
     <t>Erika Vargas</t>
   </si>
   <si>
-    <t>RTR</t>
-  </si>
-  <si>
     <t>Dailyn Gonzales</t>
-  </si>
-  <si>
-    <t>Collections</t>
   </si>
 </sst>
 </file>
@@ -339,25 +318,6 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF007A37"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -377,6 +337,25 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF007A37"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -483,18 +462,18 @@
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Resource Name"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Business Unit" dataDxfId="7">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Business Unit" dataDxfId="5">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Rate" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Hours" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Rate" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Hours" dataDxfId="3">
       <calculatedColumnFormula>SUM(OFFSET(INDIRECT(J11),0,0,1,$F$2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Subtotal" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Subtotal" dataDxfId="2">
       <calculatedColumnFormula>IFERROR(C11*D11,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Expenses" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Total" dataDxfId="2" dataCellStyle="Currency">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Expenses" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Total" dataDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>Table22[[#This Row],[Subtotal]]-Table22[[#This Row],[Expenses]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -803,7 +782,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:XFD1"/>
+      <selection pane="topRight" activeCell="B18" sqref="B18:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C1" s="15">
         <v>43399</v>
@@ -1086,8 +1065,8 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>30</v>
+      <c r="B2">
+        <v>96</v>
       </c>
       <c r="C2">
         <v>16</v>
@@ -1283,8 +1262,8 @@
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>28</v>
+      <c r="B3">
+        <v>58</v>
       </c>
       <c r="J3">
         <v>20</v>
@@ -1468,8 +1447,8 @@
       <c r="A4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>28</v>
+      <c r="B4">
+        <v>48</v>
       </c>
       <c r="W4">
         <v>40</v>
@@ -1656,8 +1635,8 @@
       <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>32</v>
+      <c r="B5">
+        <v>58</v>
       </c>
       <c r="AD5">
         <v>0</v>
@@ -1814,8 +1793,8 @@
       <c r="A6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>29</v>
+      <c r="B6">
+        <v>58</v>
       </c>
       <c r="AD6">
         <v>0</v>
@@ -1927,8 +1906,8 @@
       <c r="A7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>29</v>
+      <c r="B7">
+        <v>48</v>
       </c>
       <c r="AM7">
         <v>0</v>
@@ -2025,8 +2004,8 @@
       <c r="A8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>31</v>
+      <c r="B8">
+        <v>58</v>
       </c>
       <c r="AM8">
         <v>32</v>
@@ -2156,8 +2135,8 @@
       <c r="A9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>29</v>
+      <c r="B9">
+        <v>48</v>
       </c>
       <c r="AM9">
         <v>0</v>
@@ -2281,8 +2260,8 @@
       <c r="A10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>29</v>
+      <c r="B10">
+        <v>58</v>
       </c>
       <c r="AP10">
         <v>0</v>
@@ -2361,8 +2340,8 @@
       <c r="A11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>29</v>
+      <c r="B11">
+        <v>48</v>
       </c>
       <c r="AP11">
         <v>0</v>
@@ -2450,8 +2429,8 @@
       <c r="A12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>31</v>
+      <c r="B12">
+        <v>58</v>
       </c>
       <c r="AP12">
         <v>0</v>
@@ -2572,8 +2551,8 @@
       <c r="A13" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>33</v>
+      <c r="B13">
+        <v>58</v>
       </c>
       <c r="AP13">
         <v>0</v>
@@ -2616,8 +2595,8 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
-        <v>29</v>
+      <c r="B14">
+        <v>48</v>
       </c>
       <c r="AV14">
         <v>20</v>
@@ -2676,10 +2655,10 @@
     </row>
     <row r="15" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>58</v>
       </c>
       <c r="AZ15">
         <v>32</v>
@@ -2726,10 +2705,10 @@
     </row>
     <row r="16" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>48</v>
       </c>
       <c r="BA16">
         <v>40</v>
@@ -2752,10 +2731,10 @@
     </row>
     <row r="17" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <v>58</v>
       </c>
       <c r="BQ17">
         <v>40</v>
@@ -2775,10 +2754,10 @@
     </row>
     <row r="18" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>58</v>
       </c>
       <c r="BQ18">
         <v>40</v>
@@ -2798,10 +2777,10 @@
     </row>
     <row r="19" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>48</v>
       </c>
       <c r="BQ19">
         <v>20</v>
@@ -2821,10 +2800,10 @@
     </row>
     <row r="20" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="B20">
+        <v>58</v>
       </c>
       <c r="BQ20">
         <v>40</v>
@@ -3034,9 +3013,9 @@
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" t="str">
+      <c r="B11">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>Corporate</v>
+        <v>96</v>
       </c>
       <c r="C11" s="2">
         <v>82</v>
@@ -3068,9 +3047,9 @@
       <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B12">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>ComRes</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2">
         <v>58</v>
@@ -3102,9 +3081,9 @@
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" t="str">
+      <c r="B13">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>ComRes</v>
+        <v>48</v>
       </c>
       <c r="C13" s="2">
         <v>58</v>
@@ -3136,9 +3115,9 @@
       <c r="A14" t="s">
         <v>5</v>
       </c>
-      <c r="B14" t="str">
+      <c r="B14">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>Bill Blaise</v>
+        <v>58</v>
       </c>
       <c r="C14" s="2">
         <v>58</v>
@@ -3170,9 +3149,9 @@
       <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="B15" t="str">
+      <c r="B15">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>AutoSol</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2">
         <v>58</v>
@@ -3205,7 +3184,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2">
         <v>48</v>
@@ -3237,9 +3216,9 @@
       <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B17">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>Flow</v>
+        <v>58</v>
       </c>
       <c r="C17" s="2">
         <v>58</v>
@@ -3271,9 +3250,9 @@
       <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B18" t="str">
+      <c r="B18">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>AutoSol</v>
+        <v>48</v>
       </c>
       <c r="C18" s="2">
         <v>58</v>
@@ -3305,9 +3284,9 @@
       <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="B19" t="str">
+      <c r="B19">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>AutoSol</v>
+        <v>58</v>
       </c>
       <c r="C19" s="2">
         <v>48</v>
@@ -3339,9 +3318,9 @@
       <c r="A20" t="s">
         <v>11</v>
       </c>
-      <c r="B20" t="str">
+      <c r="B20">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>AutoSol</v>
+        <v>48</v>
       </c>
       <c r="C20" s="2">
         <v>48</v>
@@ -3373,9 +3352,9 @@
       <c r="A21" t="s">
         <v>12</v>
       </c>
-      <c r="B21" t="str">
+      <c r="B21">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>Flow</v>
+        <v>58</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2">
@@ -3405,9 +3384,9 @@
       <c r="A22" t="s">
         <v>13</v>
       </c>
-      <c r="B22" t="str">
+      <c r="B22">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>n/a</v>
+        <v>58</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2">
@@ -3437,9 +3416,9 @@
       <c r="A23" t="s">
         <v>14</v>
       </c>
-      <c r="B23" t="str">
+      <c r="B23">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>AutoSol</v>
+        <v>48</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2">
@@ -3467,11 +3446,11 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" t="str">
+        <v>29</v>
+      </c>
+      <c r="B24">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>n/a</v>
+        <v>58</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2">
@@ -3499,11 +3478,11 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" t="str">
+        <v>30</v>
+      </c>
+      <c r="B25">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>n/a</v>
+        <v>48</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2">
@@ -3531,11 +3510,11 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" t="str">
+        <v>31</v>
+      </c>
+      <c r="B26">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>RTR</v>
+        <v>58</v>
       </c>
       <c r="C26" s="2">
         <v>58</v>
@@ -3565,11 +3544,11 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" t="str">
+        <v>32</v>
+      </c>
+      <c r="B27">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>RTR</v>
+        <v>58</v>
       </c>
       <c r="C27" s="2">
         <v>58</v>
@@ -3599,11 +3578,11 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="16" t="str">
+        <v>33</v>
+      </c>
+      <c r="B28" s="16">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>Collections</v>
+        <v>48</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2">
@@ -3631,11 +3610,11 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="16" t="str">
+        <v>34</v>
+      </c>
+      <c r="B29" s="16">
         <f>IFERROR(VLOOKUP(Table22[[#This Row],[Resource Name]],Hours!A:B,2,FALSE),"")</f>
-        <v>AutoSol</v>
+        <v>58</v>
       </c>
       <c r="C29" s="2">
         <v>48</v>
@@ -3840,10 +3819,10 @@
     <mergeCell ref="D5:F7"/>
   </mergeCells>
   <conditionalFormatting sqref="G33">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>